<commit_message>
Added population and sq meters to europe JSON file
</commit_message>
<xml_diff>
--- a/maps/europe_mill_en excel template.xlsx
+++ b/maps/europe_mill_en excel template.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="12800" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="135">
   <si>
     <t>BE</t>
   </si>
@@ -64,12 +69,6 @@
   </si>
   <si>
     <t>Hungary</t>
-  </si>
-  <si>
-    <t>JO</t>
-  </si>
-  <si>
-    <t>Jordan</t>
   </si>
   <si>
     <t>DZ</t>
@@ -433,7 +432,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,6 +444,22 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Inherit"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -473,8 +488,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -491,16 +508,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -573,6 +586,12 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -584,18 +603,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:H65" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
-  <autoFilter ref="B1:H65"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:H64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B1:H64"/>
   <sortState ref="B2:G65">
     <sortCondition ref="C1:C65"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="code" dataDxfId="8"/>
-    <tableColumn id="2" name="name" dataDxfId="7"/>
-    <tableColumn id="3" name="question" dataDxfId="6"/>
-    <tableColumn id="4" name="answer" dataDxfId="5"/>
-    <tableColumn id="5" name="population" dataDxfId="4"/>
-    <tableColumn id="6" name="area" dataDxfId="3"/>
+    <tableColumn id="1" name="code" dataDxfId="6"/>
+    <tableColumn id="2" name="name" dataDxfId="5"/>
+    <tableColumn id="3" name="question" dataDxfId="4"/>
+    <tableColumn id="4" name="answer" dataDxfId="3"/>
+    <tableColumn id="5" name="population" dataDxfId="2"/>
+    <tableColumn id="6" name="area" dataDxfId="1"/>
     <tableColumn id="7" name="points" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -889,183 +908,183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H65"/>
+  <dimension ref="B1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H65" sqref="B1:H65"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="1" max="3" width="8.83203125" style="2"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8">
       <c r="B1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" ht="18" thickBot="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15" thickBot="1">
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F2" s="3">
-        <v>1000051</v>
+        <v>28007</v>
       </c>
       <c r="G2" s="2">
-        <v>1000</v>
+        <v>1580</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1">
+    <row r="3" spans="2:8" ht="15" thickBot="1">
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1000035</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1001</v>
+        <v>131</v>
+      </c>
+      <c r="F3">
+        <v>2897366</v>
+      </c>
+      <c r="G3">
+        <v>27400</v>
       </c>
       <c r="H3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1">
+    <row r="4" spans="2:8" ht="15" thickBot="1">
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1000009</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1002</v>
+        <v>131</v>
+      </c>
+      <c r="F4">
+        <v>39208194</v>
+      </c>
+      <c r="G4">
+        <v>2381740</v>
       </c>
       <c r="H4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1">
+    <row r="5" spans="2:8" ht="15" thickBot="1">
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="3">
-        <v>1000043</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1003</v>
+        <v>131</v>
+      </c>
+      <c r="F5">
+        <v>79218</v>
+      </c>
+      <c r="G5">
+        <v>470</v>
       </c>
       <c r="H5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1">
+    <row r="6" spans="2:8" ht="15" thickBot="1">
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1000024</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1004</v>
+        <v>131</v>
+      </c>
+      <c r="F6">
+        <v>8479823</v>
+      </c>
+      <c r="G6">
+        <v>82409</v>
       </c>
       <c r="H6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1">
+    <row r="7" spans="2:8" ht="15" thickBot="1">
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1000012</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1005</v>
+        <v>131</v>
+      </c>
+      <c r="F7">
+        <v>9466000</v>
+      </c>
+      <c r="G7">
+        <v>202910</v>
       </c>
       <c r="H7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1">
+    <row r="8" spans="2:8" ht="15" thickBot="1">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1073,22 +1092,22 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="3">
-        <v>1000000</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1006</v>
+        <v>131</v>
+      </c>
+      <c r="F8">
+        <v>11182817</v>
+      </c>
+      <c r="G8">
+        <v>30280</v>
       </c>
       <c r="H8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="26.25" thickBot="1">
+    <row r="9" spans="2:8" ht="40" thickBot="1">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1096,22 +1115,22 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1000006</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1007</v>
+        <v>131</v>
+      </c>
+      <c r="F9">
+        <v>3829307</v>
+      </c>
+      <c r="G9">
+        <v>51000</v>
       </c>
       <c r="H9" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1">
+    <row r="10" spans="2:8" ht="15" thickBot="1">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1119,22 +1138,22 @@
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1000002</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1008</v>
+        <v>131</v>
+      </c>
+      <c r="F10">
+        <v>7265115</v>
+      </c>
+      <c r="G10">
+        <v>108560</v>
       </c>
       <c r="H10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15.75" thickBot="1">
+    <row r="11" spans="2:8" ht="15" thickBot="1">
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1142,68 +1161,68 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1000004</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1009</v>
+        <v>131</v>
+      </c>
+      <c r="F11">
+        <v>4255700</v>
+      </c>
+      <c r="G11">
+        <v>55960</v>
       </c>
       <c r="H11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="15.75" thickBot="1">
+    <row r="12" spans="2:8" ht="15" thickBot="1">
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1000039</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1010</v>
+        <v>131</v>
+      </c>
+      <c r="F12">
+        <v>1141166</v>
+      </c>
+      <c r="G12">
+        <v>9240</v>
       </c>
       <c r="H12" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="26.25" thickBot="1">
+    <row r="13" spans="2:8" ht="27" thickBot="1">
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1000038</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1011</v>
+        <v>131</v>
+      </c>
+      <c r="F13">
+        <v>10514272</v>
+      </c>
+      <c r="G13">
+        <v>77230</v>
       </c>
       <c r="H13" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15.75" thickBot="1">
+    <row r="14" spans="2:8" ht="15" thickBot="1">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1211,114 +1230,114 @@
         <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1000003</v>
-      </c>
-      <c r="G14" s="2">
-        <v>1012</v>
+        <v>131</v>
+      </c>
+      <c r="F14">
+        <v>5614932</v>
+      </c>
+      <c r="G14">
+        <v>42430</v>
       </c>
       <c r="H14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15.75" thickBot="1">
+    <row r="15" spans="2:8" ht="15" thickBot="1">
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1000026</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1013</v>
+        <v>131</v>
+      </c>
+      <c r="F15">
+        <v>82056378</v>
+      </c>
+      <c r="G15">
+        <v>995450</v>
       </c>
       <c r="H15" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1">
+    <row r="16" spans="2:8" ht="15" thickBot="1">
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1000021</v>
-      </c>
-      <c r="G16" s="2">
-        <v>1014</v>
+        <v>131</v>
+      </c>
+      <c r="F16">
+        <v>1317997</v>
+      </c>
+      <c r="G16">
+        <v>42390</v>
       </c>
       <c r="H16" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="26.25" thickBot="1">
+    <row r="17" spans="2:8" ht="27" thickBot="1">
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1000013</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1015</v>
+        <v>131</v>
+      </c>
+      <c r="F17">
+        <v>49469</v>
+      </c>
+      <c r="G17">
+        <v>1396</v>
       </c>
       <c r="H17" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1">
+    <row r="18" spans="2:8" ht="15" thickBot="1">
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1000011</v>
-      </c>
-      <c r="G18" s="2">
-        <v>1016</v>
+        <v>131</v>
+      </c>
+      <c r="F18">
+        <v>5438972</v>
+      </c>
+      <c r="G18">
+        <v>303890</v>
       </c>
       <c r="H18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1">
+    <row r="19" spans="2:8" ht="15" thickBot="1">
       <c r="B19" s="1" t="s">
         <v>2</v>
       </c>
@@ -1326,45 +1345,45 @@
         <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1000001</v>
-      </c>
-      <c r="G19" s="2">
-        <v>1017</v>
+        <v>131</v>
+      </c>
+      <c r="F19">
+        <v>65939866</v>
+      </c>
+      <c r="G19">
+        <v>547561</v>
       </c>
       <c r="H19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15.75" thickBot="1">
+    <row r="20" spans="2:8" ht="15" thickBot="1">
       <c r="B20" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1000053</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1018</v>
+        <v>131</v>
+      </c>
+      <c r="F20">
+        <v>4487200</v>
+      </c>
+      <c r="G20">
+        <v>69490</v>
       </c>
       <c r="H20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15.75" thickBot="1">
+    <row r="21" spans="2:8" ht="15" thickBot="1">
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
@@ -1372,68 +1391,63 @@
         <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1000005</v>
-      </c>
-      <c r="G21" s="2">
-        <v>1019</v>
+        <v>131</v>
+      </c>
+      <c r="F21">
+        <v>80651873</v>
+      </c>
+      <c r="G21">
+        <v>348540</v>
       </c>
       <c r="H21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1">
+    <row r="22" spans="2:8" ht="15" thickBot="1">
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1000031</v>
-      </c>
-      <c r="G22" s="2">
-        <v>1020</v>
+        <v>131</v>
+      </c>
+      <c r="F22">
+        <v>11027549</v>
+      </c>
+      <c r="G22">
+        <v>128900</v>
       </c>
       <c r="H22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15.75" thickBot="1">
+    <row r="23" spans="2:8" ht="15" thickBot="1">
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1000037</v>
-      </c>
-      <c r="G23" s="2">
-        <v>1021</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F23" s="3"/>
       <c r="H23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15.75" thickBot="1">
+    <row r="24" spans="2:8" ht="15" thickBot="1">
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1441,321 +1455,321 @@
         <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1000007</v>
-      </c>
-      <c r="G24" s="2">
-        <v>1022</v>
+        <v>131</v>
+      </c>
+      <c r="F24">
+        <v>9893899</v>
+      </c>
+      <c r="G24">
+        <v>90530</v>
       </c>
       <c r="H24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15.75" thickBot="1">
+    <row r="25" spans="2:8" ht="15" thickBot="1">
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1000034</v>
-      </c>
-      <c r="G25" s="2">
-        <v>1023</v>
+        <v>131</v>
+      </c>
+      <c r="F25">
+        <v>323764</v>
+      </c>
+      <c r="G25">
+        <v>100250</v>
       </c>
       <c r="H25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1">
+    <row r="26" spans="2:8" ht="15" thickBot="1">
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1000033</v>
-      </c>
-      <c r="G26" s="2">
-        <v>1024</v>
+        <v>131</v>
+      </c>
+      <c r="F26">
+        <v>33417476</v>
+      </c>
+      <c r="G26">
+        <v>434320</v>
       </c>
       <c r="H26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15.75" thickBot="1">
+    <row r="27" spans="2:8" ht="15" thickBot="1">
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F27" s="3">
-        <v>1000044</v>
-      </c>
-      <c r="G27" s="2">
-        <v>1025</v>
+        <v>131</v>
+      </c>
+      <c r="F27">
+        <v>4597558</v>
+      </c>
+      <c r="G27">
+        <v>68890</v>
       </c>
       <c r="H27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="26.25" thickBot="1">
+    <row r="28" spans="2:8" ht="27" thickBot="1">
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F28" s="3">
-        <v>1000040</v>
-      </c>
-      <c r="G28" s="2">
-        <v>1026</v>
+        <v>131</v>
+      </c>
+      <c r="F28">
+        <v>85888</v>
+      </c>
+      <c r="G28">
+        <v>570</v>
       </c>
       <c r="H28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15.75" thickBot="1">
+    <row r="29" spans="2:8" ht="15" thickBot="1">
       <c r="B29" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F29" s="3">
-        <v>1000063</v>
-      </c>
-      <c r="G29" s="2">
-        <v>1027</v>
+        <v>131</v>
+      </c>
+      <c r="F29">
+        <v>8059500</v>
+      </c>
+      <c r="G29">
+        <v>21640</v>
       </c>
       <c r="H29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15.75" thickBot="1">
+    <row r="30" spans="2:8" ht="15" thickBot="1">
       <c r="B30" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" s="3">
-        <v>1000036</v>
-      </c>
-      <c r="G30" s="2">
-        <v>1028</v>
+        <v>131</v>
+      </c>
+      <c r="F30">
+        <v>60233948</v>
+      </c>
+      <c r="G30">
+        <v>294140</v>
       </c>
       <c r="H30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15.75" thickBot="1">
+    <row r="31" spans="2:8" ht="15" thickBot="1">
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F31" s="3">
-        <v>1000010</v>
+        <v>99500</v>
       </c>
       <c r="G31" s="2">
-        <v>1029</v>
+        <v>118</v>
       </c>
       <c r="H31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1">
+    <row r="32" spans="2:8" ht="15" thickBot="1">
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>132</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1000008</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1030</v>
+        <v>131</v>
+      </c>
+      <c r="F32">
+        <v>1824000</v>
+      </c>
+      <c r="G32">
+        <v>10887</v>
       </c>
       <c r="H32" s="2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" thickBot="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1">
       <c r="B33" s="1" t="s">
-        <v>134</v>
+        <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F33" s="3">
-        <v>1000055</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1031</v>
+        <v>131</v>
+      </c>
+      <c r="F33">
+        <v>2012647</v>
+      </c>
+      <c r="G33">
+        <v>62180</v>
       </c>
       <c r="H33" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="15.75" thickBot="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15" thickBot="1">
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="3">
-        <v>1000020</v>
-      </c>
-      <c r="G34" s="2">
-        <v>1032</v>
+        <v>131</v>
+      </c>
+      <c r="F34">
+        <v>4467390</v>
+      </c>
+      <c r="G34">
+        <v>10230</v>
       </c>
       <c r="H34" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="15.75" thickBot="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15" thickBot="1">
       <c r="B35" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1000015</v>
-      </c>
-      <c r="G35" s="2">
-        <v>1033</v>
+        <v>131</v>
+      </c>
+      <c r="F35">
+        <v>6201521</v>
+      </c>
+      <c r="G35">
+        <v>1759540</v>
       </c>
       <c r="H35" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" thickBot="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="27" thickBot="1">
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F36" s="3">
-        <v>1000028</v>
-      </c>
-      <c r="G36" s="2">
-        <v>1034</v>
+        <v>131</v>
+      </c>
+      <c r="F36">
+        <v>36925</v>
+      </c>
+      <c r="G36">
+        <v>160</v>
       </c>
       <c r="H36" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" ht="26.25" thickBot="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15" thickBot="1">
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F37" s="3">
-        <v>1000019</v>
-      </c>
-      <c r="G37" s="2">
-        <v>1035</v>
+        <v>131</v>
+      </c>
+      <c r="F37">
+        <v>2957689</v>
+      </c>
+      <c r="G37">
+        <v>62674</v>
       </c>
       <c r="H37" s="2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" ht="15.75" thickBot="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="27" thickBot="1">
       <c r="B38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1763,344 +1777,339 @@
         <v>45</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38">
+        <v>543360</v>
+      </c>
+      <c r="G38">
+        <v>2590</v>
+      </c>
+      <c r="H38" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="27" thickBot="1">
+      <c r="B39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39">
+        <v>2107158</v>
+      </c>
+      <c r="G39">
+        <v>25220</v>
+      </c>
+      <c r="H39" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15" thickBot="1">
+      <c r="B40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F40">
+        <v>423374</v>
+      </c>
+      <c r="G40">
+        <v>180</v>
+      </c>
+      <c r="H40" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15" thickBot="1">
+      <c r="B41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41">
+        <v>3558566</v>
+      </c>
+      <c r="G41">
+        <v>32860</v>
+      </c>
+      <c r="H41" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="27" thickBot="1">
+      <c r="B42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42">
+        <v>621383</v>
+      </c>
+      <c r="G42">
+        <v>13450</v>
+      </c>
+      <c r="H42" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="15" thickBot="1">
+      <c r="B43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F43">
+        <v>33008150</v>
+      </c>
+      <c r="G43">
+        <v>446300</v>
+      </c>
+      <c r="H43" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="27" thickBot="1">
+      <c r="B44" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F38" s="3">
-        <v>1000022</v>
-      </c>
-      <c r="G38" s="2">
-        <v>1036</v>
-      </c>
-      <c r="H38" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" ht="26.25" thickBot="1">
-      <c r="B39" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" s="3">
+        <v>3355</v>
+      </c>
+      <c r="G44" s="2">
+        <v>286257</v>
+      </c>
+      <c r="H44" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="27" thickBot="1">
+      <c r="B45" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F45">
+        <v>16804432</v>
+      </c>
+      <c r="G45">
+        <v>33720</v>
+      </c>
+      <c r="H45" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="15" thickBot="1">
+      <c r="B46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F46">
+        <v>5080166</v>
+      </c>
+      <c r="G46">
+        <v>365268</v>
+      </c>
+      <c r="H46" s="2">
         <v>46</v>
       </c>
-      <c r="C39" s="1" t="s">
+    </row>
+    <row r="47" spans="2:8" ht="15" thickBot="1">
+      <c r="B47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="H47" s="2">
         <v>47</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F39" s="3">
-        <v>1000023</v>
-      </c>
-      <c r="G39" s="2">
-        <v>1037</v>
-      </c>
-      <c r="H39" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" ht="26.25" thickBot="1">
-      <c r="B40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F40" s="3">
-        <v>1000054</v>
-      </c>
-      <c r="G40" s="2">
-        <v>1038</v>
-      </c>
-      <c r="H40" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F41" s="3">
-        <v>1000057</v>
-      </c>
-      <c r="G41" s="2">
-        <v>1039</v>
-      </c>
-      <c r="H41" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B42" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F42" s="3">
-        <v>1000047</v>
-      </c>
-      <c r="G42" s="2">
-        <v>1040</v>
-      </c>
-      <c r="H42" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" ht="26.25" thickBot="1">
-      <c r="B43" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F43" s="3">
-        <v>1000046</v>
-      </c>
-      <c r="G43" s="2">
-        <v>1041</v>
-      </c>
-      <c r="H43" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B44" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F44" s="3">
-        <v>1000050</v>
-      </c>
-      <c r="G44" s="2">
-        <v>1042</v>
-      </c>
-      <c r="H44" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" ht="26.25" thickBot="1">
-      <c r="B45" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F45" s="3">
-        <v>1000029</v>
-      </c>
-      <c r="G45" s="2">
-        <v>1043</v>
-      </c>
-      <c r="H45" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" ht="26.25" thickBot="1">
-      <c r="B46" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F46" s="3">
-        <v>1000042</v>
-      </c>
-      <c r="G46" s="2">
-        <v>1044</v>
-      </c>
-      <c r="H46" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B47" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F47" s="3">
-        <v>1000017</v>
-      </c>
-      <c r="G47" s="2">
-        <v>1045</v>
-      </c>
-      <c r="H47" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" ht="15.75" thickBot="1">
+    </row>
+    <row r="48" spans="2:8" ht="15" thickBot="1">
       <c r="B48" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1000014</v>
-      </c>
-      <c r="G48" s="2">
-        <v>1046</v>
+        <v>131</v>
+      </c>
+      <c r="F48">
+        <v>38514479</v>
+      </c>
+      <c r="G48">
+        <v>306220</v>
       </c>
       <c r="H48" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="15.75" thickBot="1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="15" thickBot="1">
       <c r="B49" s="1" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F49" s="3">
-        <v>1000027</v>
-      </c>
-      <c r="G49" s="2">
-        <v>1047</v>
+        <v>131</v>
+      </c>
+      <c r="F49">
+        <v>10457295</v>
+      </c>
+      <c r="G49">
+        <v>91590</v>
       </c>
       <c r="H49" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="15" thickBot="1">
+      <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B50" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50" s="3">
-        <v>1000016</v>
-      </c>
-      <c r="G50" s="2">
-        <v>1048</v>
+        <v>131</v>
+      </c>
+      <c r="F50">
+        <v>19981358</v>
+      </c>
+      <c r="G50">
+        <v>230020</v>
       </c>
       <c r="H50" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="15.75" thickBot="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1">
       <c r="B51" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51">
+        <v>143499861</v>
+      </c>
+      <c r="G51">
+        <v>16376870</v>
+      </c>
+      <c r="H51" s="2">
         <v>51</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F51" s="3">
-        <v>1000025</v>
-      </c>
-      <c r="G51" s="2">
-        <v>1049</v>
-      </c>
-      <c r="H51" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="15.75" thickBot="1">
+    </row>
+    <row r="52" spans="2:8" ht="27" thickBot="1">
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F52" s="3">
-        <v>1000032</v>
-      </c>
-      <c r="G52" s="2">
-        <v>1050</v>
+        <v>131</v>
+      </c>
+      <c r="F52">
+        <v>31448</v>
+      </c>
+      <c r="G52">
+        <v>60</v>
       </c>
       <c r="H52" s="2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" ht="26.25" thickBot="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="27" thickBot="1">
       <c r="B53" s="1" t="s">
         <v>116</v>
       </c>
@@ -2108,183 +2117,183 @@
         <v>117</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F53" s="3">
-        <v>1000059</v>
-      </c>
-      <c r="G53" s="2">
-        <v>1051</v>
+        <v>131</v>
+      </c>
+      <c r="F53">
+        <v>28828870</v>
+      </c>
+      <c r="G53">
+        <v>2149690</v>
       </c>
       <c r="H53" s="2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" ht="26.25" thickBot="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="15" thickBot="1">
       <c r="B54" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F54" s="3">
-        <v>1000060</v>
-      </c>
-      <c r="G54" s="2">
-        <v>1052</v>
+        <v>131</v>
+      </c>
+      <c r="F54">
+        <v>7164132</v>
+      </c>
+      <c r="G54">
+        <v>87460</v>
       </c>
       <c r="H54" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="15.75" thickBot="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="15" thickBot="1">
       <c r="B55" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F55" s="3">
-        <v>1000052</v>
-      </c>
-      <c r="G55" s="2">
-        <v>1053</v>
+        <v>131</v>
+      </c>
+      <c r="F55">
+        <v>5413393</v>
+      </c>
+      <c r="G55">
+        <v>48088</v>
       </c>
       <c r="H55" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" ht="15.75" thickBot="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="15" thickBot="1">
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F56" s="3">
-        <v>1000056</v>
-      </c>
-      <c r="G56" s="2">
-        <v>1054</v>
+        <v>131</v>
+      </c>
+      <c r="F56">
+        <v>2059953</v>
+      </c>
+      <c r="G56">
+        <v>20140</v>
       </c>
       <c r="H56" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" ht="15.75" thickBot="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="15" thickBot="1">
       <c r="B57" s="1" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1000058</v>
-      </c>
-      <c r="G57" s="2">
-        <v>1055</v>
+        <v>131</v>
+      </c>
+      <c r="F57">
+        <v>46617825</v>
+      </c>
+      <c r="G57">
+        <v>498800</v>
       </c>
       <c r="H57" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="15.75" thickBot="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="15" thickBot="1">
       <c r="B58" s="1" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1000045</v>
-      </c>
-      <c r="G58" s="2">
-        <v>1056</v>
+        <v>131</v>
+      </c>
+      <c r="F58">
+        <v>9600379</v>
+      </c>
+      <c r="G58">
+        <v>407340</v>
       </c>
       <c r="H58" s="2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="27" thickBot="1">
+      <c r="B59" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B59" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>123</v>
+        <v>58</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F59" s="3">
-        <v>1000062</v>
-      </c>
-      <c r="G59" s="2">
-        <v>1057</v>
+        <v>131</v>
+      </c>
+      <c r="F59">
+        <v>8087875</v>
+      </c>
+      <c r="G59">
+        <v>39516</v>
       </c>
       <c r="H59" s="2">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" ht="26.25" thickBot="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="15" thickBot="1">
       <c r="B60" s="1" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F60">
+        <v>22845550</v>
+      </c>
+      <c r="G60">
+        <v>183630</v>
+      </c>
+      <c r="H60" s="2">
         <v>60</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F60" s="3">
-        <v>1000030</v>
-      </c>
-      <c r="G60" s="2">
-        <v>1058</v>
-      </c>
-      <c r="H60" s="2">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" ht="15.75" thickBot="1">
+    </row>
+    <row r="61" spans="2:8" ht="15" thickBot="1">
       <c r="B61" s="1" t="s">
         <v>95</v>
       </c>
@@ -2292,119 +2301,101 @@
         <v>96</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F61" s="3">
-        <v>1000048</v>
-      </c>
-      <c r="G61" s="2">
-        <v>1059</v>
+        <v>131</v>
+      </c>
+      <c r="F61">
+        <v>10886500</v>
+      </c>
+      <c r="G61">
+        <v>155360</v>
       </c>
       <c r="H61" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" ht="15.75" thickBot="1">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="15" thickBot="1">
       <c r="B62" s="1" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F62" s="3">
-        <v>1000049</v>
-      </c>
-      <c r="G62" s="2">
-        <v>1060</v>
+        <v>131</v>
+      </c>
+      <c r="F62">
+        <v>74932641</v>
+      </c>
+      <c r="G62">
+        <v>769630</v>
       </c>
       <c r="H62" s="2">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" ht="15.75" thickBot="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="15" thickBot="1">
       <c r="B63" s="1" t="s">
-        <v>36</v>
+        <v>118</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F63" s="3">
-        <v>1000018</v>
-      </c>
-      <c r="G63" s="2">
-        <v>1061</v>
+        <v>131</v>
+      </c>
+      <c r="F63">
+        <v>45489600</v>
+      </c>
+      <c r="G63">
+        <v>579320</v>
       </c>
       <c r="H63" s="2">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B64" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>121</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="26">
+      <c r="B64" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F64" s="3">
-        <v>1000061</v>
-      </c>
-      <c r="G64" s="2">
-        <v>1062</v>
+        <v>131</v>
+      </c>
+      <c r="F64">
+        <v>64106779</v>
+      </c>
+      <c r="G64">
+        <v>241930</v>
       </c>
       <c r="H64" s="2">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8" ht="25.5">
-      <c r="B65" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F65" s="3">
-        <v>1000041</v>
-      </c>
-      <c r="G65" s="2">
-        <v>1063</v>
-      </c>
-      <c r="H65" s="2">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2414,9 +2405,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2426,8 +2422,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added flag icons to conquered countries
</commit_message>
<xml_diff>
--- a/maps/europe_mill_en excel template.xlsx
+++ b/maps/europe_mill_en excel template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="12800" windowHeight="14320"/>
+    <workbookView minimized="1" xWindow="0" yWindow="-20" windowWidth="12800" windowHeight="14320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -605,8 +605,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:H64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B1:H64"/>
-  <sortState ref="B2:G65">
-    <sortCondition ref="C1:C65"/>
+  <sortState ref="B2:H64">
+    <sortCondition ref="B1:B64"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" name="code" dataDxfId="6"/>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -948,10 +948,10 @@
     </row>
     <row r="2" spans="2:8" ht="15" thickBot="1">
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>130</v>
@@ -959,14 +959,14 @@
       <c r="E2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="3">
-        <v>28007</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1580</v>
+      <c r="F2">
+        <v>79218</v>
+      </c>
+      <c r="G2">
+        <v>470</v>
       </c>
       <c r="H2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1">
@@ -994,10 +994,10 @@
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1">
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>130</v>
@@ -1006,21 +1006,21 @@
         <v>131</v>
       </c>
       <c r="F4">
-        <v>39208194</v>
+        <v>8479823</v>
       </c>
       <c r="G4">
-        <v>2381740</v>
+        <v>82409</v>
       </c>
       <c r="H4" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1">
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>130</v>
@@ -1028,22 +1028,22 @@
       <c r="E5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F5">
-        <v>79218</v>
-      </c>
-      <c r="G5">
-        <v>470</v>
+      <c r="F5" s="3">
+        <v>28007</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1580</v>
       </c>
       <c r="H5" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1">
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>130</v>
@@ -1052,21 +1052,21 @@
         <v>131</v>
       </c>
       <c r="F6">
-        <v>8479823</v>
+        <v>3829307</v>
       </c>
       <c r="G6">
-        <v>82409</v>
+        <v>51000</v>
       </c>
       <c r="H6" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>130</v>
@@ -1075,21 +1075,21 @@
         <v>131</v>
       </c>
       <c r="F7">
-        <v>9466000</v>
+        <v>11182817</v>
       </c>
       <c r="G7">
-        <v>202910</v>
+        <v>30280</v>
       </c>
       <c r="H7" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1">
       <c r="B8" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>130</v>
@@ -1098,21 +1098,21 @@
         <v>131</v>
       </c>
       <c r="F8">
-        <v>11182817</v>
+        <v>7265115</v>
       </c>
       <c r="G8">
-        <v>30280</v>
+        <v>108560</v>
       </c>
       <c r="H8" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="40" thickBot="1">
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>130</v>
@@ -1121,21 +1121,21 @@
         <v>131</v>
       </c>
       <c r="F9">
-        <v>3829307</v>
+        <v>9466000</v>
       </c>
       <c r="G9">
-        <v>51000</v>
+        <v>202910</v>
       </c>
       <c r="H9" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15" thickBot="1">
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>130</v>
@@ -1144,21 +1144,21 @@
         <v>131</v>
       </c>
       <c r="F10">
-        <v>7265115</v>
+        <v>8087875</v>
       </c>
       <c r="G10">
-        <v>108560</v>
+        <v>39516</v>
       </c>
       <c r="H10" s="2">
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1">
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>130</v>
@@ -1167,21 +1167,21 @@
         <v>131</v>
       </c>
       <c r="F11">
-        <v>4255700</v>
+        <v>1141166</v>
       </c>
       <c r="G11">
-        <v>55960</v>
+        <v>9240</v>
       </c>
       <c r="H11" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15" thickBot="1">
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>130</v>
@@ -1190,21 +1190,21 @@
         <v>131</v>
       </c>
       <c r="F12">
-        <v>1141166</v>
+        <v>10514272</v>
       </c>
       <c r="G12">
-        <v>9240</v>
+        <v>77230</v>
       </c>
       <c r="H12" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="27" thickBot="1">
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>130</v>
@@ -1213,13 +1213,13 @@
         <v>131</v>
       </c>
       <c r="F13">
-        <v>10514272</v>
+        <v>80651873</v>
       </c>
       <c r="G13">
-        <v>77230</v>
+        <v>348540</v>
       </c>
       <c r="H13" s="2">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15" thickBot="1">
@@ -1247,10 +1247,10 @@
     </row>
     <row r="15" spans="2:8" ht="15" thickBot="1">
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>130</v>
@@ -1259,13 +1259,13 @@
         <v>131</v>
       </c>
       <c r="F15">
-        <v>82056378</v>
+        <v>39208194</v>
       </c>
       <c r="G15">
-        <v>995450</v>
+        <v>2381740</v>
       </c>
       <c r="H15" s="2">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="15" thickBot="1">
@@ -1293,10 +1293,10 @@
     </row>
     <row r="17" spans="2:8" ht="27" thickBot="1">
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>130</v>
@@ -1305,21 +1305,21 @@
         <v>131</v>
       </c>
       <c r="F17">
-        <v>49469</v>
+        <v>82056378</v>
       </c>
       <c r="G17">
-        <v>1396</v>
+        <v>995450</v>
       </c>
       <c r="H17" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1">
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>130</v>
@@ -1328,21 +1328,21 @@
         <v>131</v>
       </c>
       <c r="F18">
-        <v>5438972</v>
+        <v>46617825</v>
       </c>
       <c r="G18">
-        <v>303890</v>
+        <v>498800</v>
       </c>
       <c r="H18" s="2">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15" thickBot="1">
       <c r="B19" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>130</v>
@@ -1351,21 +1351,21 @@
         <v>131</v>
       </c>
       <c r="F19">
-        <v>65939866</v>
+        <v>5438972</v>
       </c>
       <c r="G19">
-        <v>547561</v>
+        <v>303890</v>
       </c>
       <c r="H19" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15" thickBot="1">
       <c r="B20" s="1" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>130</v>
@@ -1374,21 +1374,21 @@
         <v>131</v>
       </c>
       <c r="F20">
-        <v>4487200</v>
+        <v>49469</v>
       </c>
       <c r="G20">
-        <v>69490</v>
+        <v>1396</v>
       </c>
       <c r="H20" s="2">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15" thickBot="1">
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>130</v>
@@ -1397,21 +1397,21 @@
         <v>131</v>
       </c>
       <c r="F21">
-        <v>80651873</v>
+        <v>65939866</v>
       </c>
       <c r="G21">
-        <v>348540</v>
+        <v>547561</v>
       </c>
       <c r="H21" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15" thickBot="1">
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>130</v>
@@ -1420,21 +1420,21 @@
         <v>131</v>
       </c>
       <c r="F22">
-        <v>11027549</v>
+        <v>64106779</v>
       </c>
       <c r="G22">
-        <v>128900</v>
+        <v>241930</v>
       </c>
       <c r="H22" s="2">
-        <v>21</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15" thickBot="1">
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>130</v>
@@ -1442,17 +1442,22 @@
       <c r="E23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23">
+        <v>4487200</v>
+      </c>
+      <c r="G23">
+        <v>69490</v>
+      </c>
       <c r="H23" s="2">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15" thickBot="1">
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>130</v>
@@ -1460,22 +1465,17 @@
       <c r="E24" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F24">
-        <v>9893899</v>
-      </c>
-      <c r="G24">
-        <v>90530</v>
-      </c>
+      <c r="F24" s="3"/>
       <c r="H24" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15" thickBot="1">
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>130</v>
@@ -1484,21 +1484,21 @@
         <v>131</v>
       </c>
       <c r="F25">
-        <v>323764</v>
+        <v>11027549</v>
       </c>
       <c r="G25">
-        <v>100250</v>
+        <v>128900</v>
       </c>
       <c r="H25" s="2">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15" thickBot="1">
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>130</v>
@@ -1507,21 +1507,21 @@
         <v>131</v>
       </c>
       <c r="F26">
-        <v>33417476</v>
+        <v>4255700</v>
       </c>
       <c r="G26">
-        <v>434320</v>
+        <v>55960</v>
       </c>
       <c r="H26" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15" thickBot="1">
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>86</v>
+        <v>15</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>130</v>
@@ -1530,21 +1530,21 @@
         <v>131</v>
       </c>
       <c r="F27">
-        <v>4597558</v>
+        <v>9893899</v>
       </c>
       <c r="G27">
-        <v>68890</v>
+        <v>90530</v>
       </c>
       <c r="H27" s="2">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="27" thickBot="1">
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>130</v>
@@ -1553,13 +1553,13 @@
         <v>131</v>
       </c>
       <c r="F28">
-        <v>85888</v>
+        <v>4597558</v>
       </c>
       <c r="G28">
-        <v>570</v>
+        <v>68890</v>
       </c>
       <c r="H28" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15" thickBot="1">
@@ -1587,10 +1587,10 @@
     </row>
     <row r="30" spans="2:8" ht="15" thickBot="1">
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>130</v>
@@ -1599,21 +1599,21 @@
         <v>131</v>
       </c>
       <c r="F30">
-        <v>60233948</v>
+        <v>85888</v>
       </c>
       <c r="G30">
-        <v>294140</v>
+        <v>570</v>
       </c>
       <c r="H30" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15" thickBot="1">
       <c r="B31" s="1" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>130</v>
@@ -1621,22 +1621,22 @@
       <c r="E31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="3">
-        <v>99500</v>
-      </c>
-      <c r="G31" s="2">
-        <v>118</v>
+      <c r="F31">
+        <v>33417476</v>
+      </c>
+      <c r="G31">
+        <v>434320</v>
       </c>
       <c r="H31" s="2">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" thickBot="1">
       <c r="B32" s="1" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>130</v>
@@ -1645,21 +1645,21 @@
         <v>131</v>
       </c>
       <c r="F32">
-        <v>1824000</v>
+        <v>323764</v>
       </c>
       <c r="G32">
-        <v>10887</v>
+        <v>100250</v>
       </c>
       <c r="H32" s="2">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="15" thickBot="1">
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>130</v>
@@ -1668,21 +1668,21 @@
         <v>131</v>
       </c>
       <c r="F33">
-        <v>2012647</v>
+        <v>60233948</v>
       </c>
       <c r="G33">
-        <v>62180</v>
+        <v>294140</v>
       </c>
       <c r="H33" s="2">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:8" ht="15" thickBot="1">
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>130</v>
@@ -1690,22 +1690,22 @@
       <c r="E34" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F34">
-        <v>4467390</v>
-      </c>
-      <c r="G34">
-        <v>10230</v>
+      <c r="F34" s="3">
+        <v>99500</v>
+      </c>
+      <c r="G34" s="2">
+        <v>118</v>
       </c>
       <c r="H34" s="2">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:8" ht="15" thickBot="1">
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>130</v>
@@ -1714,13 +1714,13 @@
         <v>131</v>
       </c>
       <c r="F35">
-        <v>6201521</v>
+        <v>4467390</v>
       </c>
       <c r="G35">
-        <v>1759540</v>
+        <v>10230</v>
       </c>
       <c r="H35" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="27" thickBot="1">
@@ -1794,10 +1794,10 @@
     </row>
     <row r="39" spans="2:8" ht="27" thickBot="1">
       <c r="B39" s="1" t="s">
-        <v>105</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>130</v>
@@ -1806,21 +1806,21 @@
         <v>131</v>
       </c>
       <c r="F39">
-        <v>2107158</v>
+        <v>2012647</v>
       </c>
       <c r="G39">
-        <v>25220</v>
+        <v>62180</v>
       </c>
       <c r="H39" s="2">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="2:8" ht="15" thickBot="1">
       <c r="B40" s="1" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>130</v>
@@ -1829,21 +1829,21 @@
         <v>131</v>
       </c>
       <c r="F40">
-        <v>423374</v>
+        <v>6201521</v>
       </c>
       <c r="G40">
-        <v>180</v>
+        <v>1759540</v>
       </c>
       <c r="H40" s="2">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="15" thickBot="1">
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>130</v>
@@ -1852,21 +1852,21 @@
         <v>131</v>
       </c>
       <c r="F41">
-        <v>3558566</v>
+        <v>33008150</v>
       </c>
       <c r="G41">
-        <v>32860</v>
+        <v>446300</v>
       </c>
       <c r="H41" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="27" thickBot="1">
       <c r="B42" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>130</v>
@@ -1875,21 +1875,21 @@
         <v>131</v>
       </c>
       <c r="F42">
-        <v>621383</v>
+        <v>3558566</v>
       </c>
       <c r="G42">
-        <v>13450</v>
+        <v>32860</v>
       </c>
       <c r="H42" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:8" ht="15" thickBot="1">
       <c r="B43" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>130</v>
@@ -1898,21 +1898,21 @@
         <v>131</v>
       </c>
       <c r="F43">
-        <v>33008150</v>
+        <v>621383</v>
       </c>
       <c r="G43">
-        <v>446300</v>
+        <v>13450</v>
       </c>
       <c r="H43" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="2:8" ht="27" thickBot="1">
       <c r="B44" s="1" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>130</v>
@@ -1920,22 +1920,22 @@
       <c r="E44" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F44" s="3">
-        <v>3355</v>
-      </c>
-      <c r="G44" s="2">
-        <v>286257</v>
+      <c r="F44">
+        <v>2107158</v>
+      </c>
+      <c r="G44">
+        <v>25220</v>
       </c>
       <c r="H44" s="2">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:8" ht="27" thickBot="1">
       <c r="B45" s="1" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>130</v>
@@ -1944,21 +1944,21 @@
         <v>131</v>
       </c>
       <c r="F45">
-        <v>16804432</v>
+        <v>423374</v>
       </c>
       <c r="G45">
-        <v>33720</v>
+        <v>180</v>
       </c>
       <c r="H45" s="2">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:8" ht="15" thickBot="1">
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>130</v>
@@ -1966,22 +1966,22 @@
       <c r="E46" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F46">
-        <v>5080166</v>
-      </c>
-      <c r="G46">
-        <v>365268</v>
+      <c r="F46" s="3">
+        <v>3355</v>
+      </c>
+      <c r="G46" s="2">
+        <v>286257</v>
       </c>
       <c r="H46" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="15" thickBot="1">
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>130</v>
@@ -1989,17 +1989,22 @@
       <c r="E47" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F47" s="3"/>
+      <c r="F47">
+        <v>16804432</v>
+      </c>
+      <c r="G47">
+        <v>33720</v>
+      </c>
       <c r="H47" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="2:8" ht="15" thickBot="1">
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>130</v>
@@ -2008,21 +2013,21 @@
         <v>131</v>
       </c>
       <c r="F48">
-        <v>38514479</v>
+        <v>5080166</v>
       </c>
       <c r="G48">
-        <v>306220</v>
+        <v>365268</v>
       </c>
       <c r="H48" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="2:8" ht="15" thickBot="1">
       <c r="B49" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>130</v>
@@ -2031,21 +2036,21 @@
         <v>131</v>
       </c>
       <c r="F49">
-        <v>10457295</v>
+        <v>38514479</v>
       </c>
       <c r="G49">
-        <v>91590</v>
+        <v>306220</v>
       </c>
       <c r="H49" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="15" thickBot="1">
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>130</v>
@@ -2053,22 +2058,17 @@
       <c r="E50" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F50">
-        <v>19981358</v>
-      </c>
-      <c r="G50">
-        <v>230020</v>
-      </c>
+      <c r="F50" s="3"/>
       <c r="H50" s="2">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="15" thickBot="1">
       <c r="B51" s="1" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>130</v>
@@ -2077,21 +2077,21 @@
         <v>131</v>
       </c>
       <c r="F51">
-        <v>143499861</v>
+        <v>10457295</v>
       </c>
       <c r="G51">
-        <v>16376870</v>
+        <v>91590</v>
       </c>
       <c r="H51" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:8" ht="27" thickBot="1">
       <c r="B52" s="1" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>130</v>
@@ -2100,21 +2100,21 @@
         <v>131</v>
       </c>
       <c r="F52">
-        <v>31448</v>
+        <v>19981358</v>
       </c>
       <c r="G52">
-        <v>60</v>
+        <v>230020</v>
       </c>
       <c r="H52" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:8" ht="27" thickBot="1">
       <c r="B53" s="1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>130</v>
@@ -2123,21 +2123,21 @@
         <v>131</v>
       </c>
       <c r="F53">
-        <v>28828870</v>
+        <v>7164132</v>
       </c>
       <c r="G53">
-        <v>2149690</v>
+        <v>87460</v>
       </c>
       <c r="H53" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="2:8" ht="15" thickBot="1">
       <c r="B54" s="1" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>130</v>
@@ -2146,21 +2146,21 @@
         <v>131</v>
       </c>
       <c r="F54">
-        <v>7164132</v>
+        <v>143499861</v>
       </c>
       <c r="G54">
-        <v>87460</v>
+        <v>16376870</v>
       </c>
       <c r="H54" s="2">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="15" thickBot="1">
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>130</v>
@@ -2169,21 +2169,21 @@
         <v>131</v>
       </c>
       <c r="F55">
-        <v>5413393</v>
+        <v>28828870</v>
       </c>
       <c r="G55">
-        <v>48088</v>
+        <v>2149690</v>
       </c>
       <c r="H55" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="15" thickBot="1">
       <c r="B56" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>130</v>
@@ -2192,21 +2192,21 @@
         <v>131</v>
       </c>
       <c r="F56">
-        <v>2059953</v>
+        <v>9600379</v>
       </c>
       <c r="G56">
-        <v>20140</v>
+        <v>407340</v>
       </c>
       <c r="H56" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="2:8" ht="15" thickBot="1">
       <c r="B57" s="1" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>130</v>
@@ -2215,21 +2215,21 @@
         <v>131</v>
       </c>
       <c r="F57">
-        <v>46617825</v>
+        <v>2059953</v>
       </c>
       <c r="G57">
-        <v>498800</v>
+        <v>20140</v>
       </c>
       <c r="H57" s="2">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="2:8" ht="15" thickBot="1">
       <c r="B58" s="1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>130</v>
@@ -2238,21 +2238,21 @@
         <v>131</v>
       </c>
       <c r="F58">
-        <v>9600379</v>
+        <v>5413393</v>
       </c>
       <c r="G58">
-        <v>407340</v>
+        <v>48088</v>
       </c>
       <c r="H58" s="2">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="27" thickBot="1">
       <c r="B59" s="1" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>130</v>
@@ -2261,13 +2261,13 @@
         <v>131</v>
       </c>
       <c r="F59">
-        <v>8087875</v>
+        <v>31448</v>
       </c>
       <c r="G59">
-        <v>39516</v>
+        <v>60</v>
       </c>
       <c r="H59" s="2">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="2:8" ht="15" thickBot="1">
@@ -2364,10 +2364,10 @@
     </row>
     <row r="64" spans="2:8" ht="26">
       <c r="B64" s="4" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>130</v>
@@ -2376,13 +2376,13 @@
         <v>131</v>
       </c>
       <c r="F64">
-        <v>64106779</v>
+        <v>1824000</v>
       </c>
       <c r="G64">
-        <v>241930</v>
+        <v>10887</v>
       </c>
       <c r="H64" s="2">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added multiple choice answers
</commit_message>
<xml_diff>
--- a/maps/europe_mill_en excel template.xlsx
+++ b/maps/europe_mill_en excel template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="-20" windowWidth="12800" windowHeight="14320"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="142">
   <si>
     <t>BE</t>
   </si>
@@ -426,6 +426,27 @@
   </si>
   <si>
     <t>points</t>
+  </si>
+  <si>
+    <t>Whar's the name of a famous statue in Antwerp</t>
+  </si>
+  <si>
+    <t>Manneken Pis</t>
+  </si>
+  <si>
+    <t>Why?</t>
+  </si>
+  <si>
+    <t>answer-2</t>
+  </si>
+  <si>
+    <t>answer-3</t>
+  </si>
+  <si>
+    <t>Eifel tower</t>
+  </si>
+  <si>
+    <t>Christ the Redeemer</t>
   </si>
 </sst>
 </file>
@@ -488,8 +509,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -508,12 +539,22 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -522,6 +563,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -603,16 +650,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:H64" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="B1:H64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:J64" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="B1:J64"/>
   <sortState ref="B2:H64">
     <sortCondition ref="B1:B64"/>
   </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" name="code" dataDxfId="6"/>
-    <tableColumn id="2" name="name" dataDxfId="5"/>
-    <tableColumn id="3" name="question" dataDxfId="4"/>
-    <tableColumn id="4" name="answer" dataDxfId="3"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="code" dataDxfId="8"/>
+    <tableColumn id="2" name="name" dataDxfId="7"/>
+    <tableColumn id="3" name="question" dataDxfId="6"/>
+    <tableColumn id="4" name="answer" dataDxfId="5"/>
+    <tableColumn id="10" name="answer-2" dataDxfId="4"/>
+    <tableColumn id="9" name="answer-3" dataDxfId="3"/>
     <tableColumn id="5" name="population" dataDxfId="2"/>
     <tableColumn id="6" name="area" dataDxfId="1"/>
     <tableColumn id="7" name="points" dataDxfId="0"/>
@@ -908,22 +957,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H64"/>
+  <dimension ref="B1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="2"/>
-    <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="2" width="8.83203125" style="2"/>
+    <col min="3" max="3" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="2:10">
       <c r="B1" s="2" t="s">
         <v>124</v>
       </c>
@@ -937,16 +989,22 @@
         <v>127</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="15" thickBot="1">
+    <row r="2" spans="2:10" ht="15" thickBot="1">
       <c r="B2" s="1" t="s">
         <v>83</v>
       </c>
@@ -959,17 +1017,23 @@
       <c r="E2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2">
         <v>79218</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>470</v>
       </c>
-      <c r="H2" s="2">
+      <c r="J2" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15" thickBot="1">
+    <row r="3" spans="2:10" ht="15" thickBot="1">
       <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
@@ -982,17 +1046,23 @@
       <c r="E3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3">
         <v>2897366</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>27400</v>
       </c>
-      <c r="H3" s="2">
+      <c r="J3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1">
+    <row r="4" spans="2:10" ht="15" thickBot="1">
       <c r="B4" s="1" t="s">
         <v>46</v>
       </c>
@@ -1005,17 +1075,23 @@
       <c r="E4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4">
         <v>8479823</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>82409</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1">
+    <row r="5" spans="2:10" ht="15" thickBot="1">
       <c r="B5" s="1" t="s">
         <v>99</v>
       </c>
@@ -1028,17 +1104,23 @@
       <c r="E5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5" s="3">
         <v>28007</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>1580</v>
       </c>
-      <c r="H5" s="2">
+      <c r="J5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1">
+    <row r="6" spans="2:10" ht="27" thickBot="1">
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1051,17 +1133,23 @@
       <c r="E6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6">
         <v>3829307</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>51000</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1">
+    <row r="7" spans="2:10" ht="15" thickBot="1">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,22 +1157,28 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F7">
+        <v>136</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7">
         <v>11182817</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>30280</v>
       </c>
-      <c r="H7" s="2">
+      <c r="J7" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1">
+    <row r="8" spans="2:10" ht="15" thickBot="1">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1097,17 +1191,23 @@
       <c r="E8" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8">
         <v>7265115</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>108560</v>
       </c>
-      <c r="H8" s="2">
+      <c r="J8" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="40" thickBot="1">
+    <row r="9" spans="2:10" ht="15" thickBot="1">
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1120,17 +1220,23 @@
       <c r="E9" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9">
         <v>9466000</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>202910</v>
       </c>
-      <c r="H9" s="2">
+      <c r="J9" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="15" thickBot="1">
+    <row r="10" spans="2:10" ht="15" thickBot="1">
       <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1138,22 +1244,28 @@
         <v>58</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10">
         <v>8087875</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>39516</v>
       </c>
-      <c r="H10" s="2">
+      <c r="J10" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="15" thickBot="1">
+    <row r="11" spans="2:10" ht="15" thickBot="1">
       <c r="B11" s="1" t="s">
         <v>75</v>
       </c>
@@ -1166,17 +1278,23 @@
       <c r="E11" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11">
         <v>1141166</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>9240</v>
       </c>
-      <c r="H11" s="2">
+      <c r="J11" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="15" thickBot="1">
+    <row r="12" spans="2:10" ht="15" thickBot="1">
       <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
@@ -1189,17 +1307,23 @@
       <c r="E12" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H12">
         <v>10514272</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>77230</v>
       </c>
-      <c r="H12" s="2">
+      <c r="J12" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="27" thickBot="1">
+    <row r="13" spans="2:10" ht="15" thickBot="1">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1212,17 +1336,23 @@
       <c r="E13" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H13">
         <v>80651873</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>348540</v>
       </c>
-      <c r="H13" s="2">
+      <c r="J13" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="15" thickBot="1">
+    <row r="14" spans="2:10" ht="15" thickBot="1">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1235,17 +1365,23 @@
       <c r="E14" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14">
         <v>5614932</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>42430</v>
       </c>
-      <c r="H14" s="2">
+      <c r="J14" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="15" thickBot="1">
+    <row r="15" spans="2:10" ht="15" thickBot="1">
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1258,17 +1394,23 @@
       <c r="E15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H15">
         <v>39208194</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>2381740</v>
       </c>
-      <c r="H15" s="2">
+      <c r="J15" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="15" thickBot="1">
+    <row r="16" spans="2:10" ht="15" thickBot="1">
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1281,17 +1423,23 @@
       <c r="E16" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16">
         <v>1317997</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>42390</v>
       </c>
-      <c r="H16" s="2">
+      <c r="J16" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="27" thickBot="1">
+    <row r="17" spans="2:10" ht="15" thickBot="1">
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -1304,17 +1452,23 @@
       <c r="E17" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H17">
         <v>82056378</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>995450</v>
       </c>
-      <c r="H17" s="2">
+      <c r="J17" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1">
+    <row r="18" spans="2:10" ht="15" thickBot="1">
       <c r="B18" s="1" t="s">
         <v>87</v>
       </c>
@@ -1327,17 +1481,23 @@
       <c r="E18" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H18">
         <v>46617825</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>498800</v>
       </c>
-      <c r="H18" s="2">
+      <c r="J18" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15" thickBot="1">
+    <row r="19" spans="2:10" ht="15" thickBot="1">
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1350,17 +1510,23 @@
       <c r="E19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19">
         <v>5438972</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>303890</v>
       </c>
-      <c r="H19" s="2">
+      <c r="J19" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="15" thickBot="1">
+    <row r="20" spans="2:10" ht="15" thickBot="1">
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1373,17 +1539,23 @@
       <c r="E20" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H20">
         <v>49469</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>1396</v>
       </c>
-      <c r="H20" s="2">
+      <c r="J20" s="2">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15" thickBot="1">
+    <row r="21" spans="2:10" ht="15" thickBot="1">
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
@@ -1396,17 +1568,23 @@
       <c r="E21" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H21">
         <v>65939866</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>547561</v>
       </c>
-      <c r="H21" s="2">
+      <c r="J21" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="15" thickBot="1">
+    <row r="22" spans="2:10" ht="27" thickBot="1">
       <c r="B22" s="1" t="s">
         <v>79</v>
       </c>
@@ -1419,17 +1597,23 @@
       <c r="E22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22">
         <v>64106779</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>241930</v>
       </c>
-      <c r="H22" s="2">
+      <c r="J22" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="15" thickBot="1">
+    <row r="23" spans="2:10" ht="15" thickBot="1">
       <c r="B23" s="1" t="s">
         <v>103</v>
       </c>
@@ -1442,17 +1626,23 @@
       <c r="E23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23">
         <v>4487200</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>69490</v>
       </c>
-      <c r="H23" s="2">
+      <c r="J23" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="15" thickBot="1">
+    <row r="24" spans="2:10" ht="15" thickBot="1">
       <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
@@ -1465,12 +1655,18 @@
       <c r="E24" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="H24" s="2">
+      <c r="F24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="J24" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="15" thickBot="1">
+    <row r="25" spans="2:10" ht="15" thickBot="1">
       <c r="B25" s="1" t="s">
         <v>59</v>
       </c>
@@ -1483,17 +1679,23 @@
       <c r="E25" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25">
         <v>11027549</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>128900</v>
       </c>
-      <c r="H25" s="2">
+      <c r="J25" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15" thickBot="1">
+    <row r="26" spans="2:10" ht="15" thickBot="1">
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
@@ -1506,17 +1708,23 @@
       <c r="E26" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26">
         <v>4255700</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>55960</v>
       </c>
-      <c r="H26" s="2">
+      <c r="J26" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="15" thickBot="1">
+    <row r="27" spans="2:10" ht="15" thickBot="1">
       <c r="B27" s="1" t="s">
         <v>14</v>
       </c>
@@ -1529,17 +1737,23 @@
       <c r="E27" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27">
         <v>9893899</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>90530</v>
       </c>
-      <c r="H27" s="2">
+      <c r="J27" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="27" thickBot="1">
+    <row r="28" spans="2:10" ht="15" thickBot="1">
       <c r="B28" s="1" t="s">
         <v>85</v>
       </c>
@@ -1552,17 +1766,23 @@
       <c r="E28" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28">
         <v>4597558</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>68890</v>
       </c>
-      <c r="H28" s="2">
+      <c r="J28" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15" thickBot="1">
+    <row r="29" spans="2:10" ht="15" thickBot="1">
       <c r="B29" s="1" t="s">
         <v>122</v>
       </c>
@@ -1575,17 +1795,23 @@
       <c r="E29" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29">
         <v>8059500</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>21640</v>
       </c>
-      <c r="H29" s="2">
+      <c r="J29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15" thickBot="1">
+    <row r="30" spans="2:10" ht="15" thickBot="1">
       <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
@@ -1598,17 +1824,23 @@
       <c r="E30" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H30">
         <v>85888</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>570</v>
       </c>
-      <c r="H30" s="2">
+      <c r="J30" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="15" thickBot="1">
+    <row r="31" spans="2:10" ht="15" thickBot="1">
       <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
@@ -1621,17 +1853,23 @@
       <c r="E31" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31">
         <v>33417476</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <v>434320</v>
       </c>
-      <c r="H31" s="2">
+      <c r="J31" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="15" thickBot="1">
+    <row r="32" spans="2:10" ht="15" thickBot="1">
       <c r="B32" s="1" t="s">
         <v>65</v>
       </c>
@@ -1644,17 +1882,23 @@
       <c r="E32" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32">
         <v>323764</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <v>100250</v>
       </c>
-      <c r="H32" s="2">
+      <c r="J32" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1">
+    <row r="33" spans="2:10" ht="15" thickBot="1">
       <c r="B33" s="1" t="s">
         <v>69</v>
       </c>
@@ -1667,17 +1911,23 @@
       <c r="E33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H33">
         <v>60233948</v>
       </c>
-      <c r="G33">
+      <c r="I33">
         <v>294140</v>
       </c>
-      <c r="H33" s="2">
+      <c r="J33" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="15" thickBot="1">
+    <row r="34" spans="2:10" ht="15" thickBot="1">
       <c r="B34" s="1" t="s">
         <v>18</v>
       </c>
@@ -1690,17 +1940,23 @@
       <c r="E34" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H34" s="3">
         <v>99500</v>
       </c>
-      <c r="G34" s="2">
+      <c r="I34" s="2">
         <v>118</v>
       </c>
-      <c r="H34" s="2">
+      <c r="J34" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="15" thickBot="1">
+    <row r="35" spans="2:10" ht="15" thickBot="1">
       <c r="B35" s="1" t="s">
         <v>28</v>
       </c>
@@ -1713,17 +1969,23 @@
       <c r="E35" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H35">
         <v>4467390</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <v>10230</v>
       </c>
-      <c r="H35" s="2">
+      <c r="J35" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="27" thickBot="1">
+    <row r="36" spans="2:10" ht="27" thickBot="1">
       <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
@@ -1736,17 +1998,23 @@
       <c r="E36" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H36">
         <v>36925</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <v>160</v>
       </c>
-      <c r="H36" s="2">
+      <c r="J36" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15" thickBot="1">
+    <row r="37" spans="2:10" ht="15" thickBot="1">
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1759,17 +2027,23 @@
       <c r="E37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H37">
         <v>2957689</v>
       </c>
-      <c r="G37">
+      <c r="I37">
         <v>62674</v>
       </c>
-      <c r="H37" s="2">
+      <c r="J37" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="27" thickBot="1">
+    <row r="38" spans="2:10" ht="27" thickBot="1">
       <c r="B38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1782,17 +2056,23 @@
       <c r="E38" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38">
         <v>543360</v>
       </c>
-      <c r="G38">
+      <c r="I38">
         <v>2590</v>
       </c>
-      <c r="H38" s="2">
+      <c r="J38" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="27" thickBot="1">
+    <row r="39" spans="2:10" ht="15" thickBot="1">
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1805,17 +2085,23 @@
       <c r="E39" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H39">
         <v>2012647</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <v>62180</v>
       </c>
-      <c r="H39" s="2">
+      <c r="J39" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="15" thickBot="1">
+    <row r="40" spans="2:10" ht="15" thickBot="1">
       <c r="B40" s="1" t="s">
         <v>54</v>
       </c>
@@ -1828,17 +2114,23 @@
       <c r="E40" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40">
         <v>6201521</v>
       </c>
-      <c r="G40">
+      <c r="I40">
         <v>1759540</v>
       </c>
-      <c r="H40" s="2">
+      <c r="J40" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15" thickBot="1">
+    <row r="41" spans="2:10" ht="15" thickBot="1">
       <c r="B41" s="1" t="s">
         <v>97</v>
       </c>
@@ -1851,17 +2143,23 @@
       <c r="E41" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H41">
         <v>33008150</v>
       </c>
-      <c r="G41">
+      <c r="I41">
         <v>446300</v>
       </c>
-      <c r="H41" s="2">
+      <c r="J41" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="27" thickBot="1">
+    <row r="42" spans="2:10" ht="15" thickBot="1">
       <c r="B42" s="1" t="s">
         <v>91</v>
       </c>
@@ -1874,17 +2172,23 @@
       <c r="E42" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H42">
         <v>3558566</v>
       </c>
-      <c r="G42">
+      <c r="I42">
         <v>32860</v>
       </c>
-      <c r="H42" s="2">
+      <c r="J42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="15" thickBot="1">
+    <row r="43" spans="2:10" ht="27" thickBot="1">
       <c r="B43" s="1" t="s">
         <v>89</v>
       </c>
@@ -1897,17 +2201,23 @@
       <c r="E43" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H43">
         <v>621383</v>
       </c>
-      <c r="G43">
+      <c r="I43">
         <v>13450</v>
       </c>
-      <c r="H43" s="2">
+      <c r="J43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="27" thickBot="1">
+    <row r="44" spans="2:10" ht="15" thickBot="1">
       <c r="B44" s="1" t="s">
         <v>105</v>
       </c>
@@ -1920,17 +2230,23 @@
       <c r="E44" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H44">
         <v>2107158</v>
       </c>
-      <c r="G44">
+      <c r="I44">
         <v>25220</v>
       </c>
-      <c r="H44" s="2">
+      <c r="J44" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="27" thickBot="1">
+    <row r="45" spans="2:10" ht="15" thickBot="1">
       <c r="B45" s="1" t="s">
         <v>110</v>
       </c>
@@ -1943,17 +2259,23 @@
       <c r="E45" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H45">
         <v>423374</v>
       </c>
-      <c r="G45">
+      <c r="I45">
         <v>180</v>
       </c>
-      <c r="H45" s="2">
+      <c r="J45" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="15" thickBot="1">
+    <row r="46" spans="2:10" ht="15" thickBot="1">
       <c r="B46" s="1" t="s">
         <v>133</v>
       </c>
@@ -1966,17 +2288,23 @@
       <c r="E46" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H46" s="3">
         <v>3355</v>
       </c>
-      <c r="G46" s="2">
+      <c r="I46" s="2">
         <v>286257</v>
       </c>
-      <c r="H46" s="2">
+      <c r="J46" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="15" thickBot="1">
+    <row r="47" spans="2:10" ht="27" thickBot="1">
       <c r="B47" s="1" t="s">
         <v>81</v>
       </c>
@@ -1989,17 +2317,23 @@
       <c r="E47" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H47">
         <v>16804432</v>
       </c>
-      <c r="G47">
+      <c r="I47">
         <v>33720</v>
       </c>
-      <c r="H47" s="2">
+      <c r="J47" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="15" thickBot="1">
+    <row r="48" spans="2:10" ht="15" thickBot="1">
       <c r="B48" s="1" t="s">
         <v>32</v>
       </c>
@@ -2012,17 +2346,23 @@
       <c r="E48" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H48">
         <v>5080166</v>
       </c>
-      <c r="G48">
+      <c r="I48">
         <v>365268</v>
       </c>
-      <c r="H48" s="2">
+      <c r="J48" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="15" thickBot="1">
+    <row r="49" spans="2:10" ht="15" thickBot="1">
       <c r="B49" s="1" t="s">
         <v>52</v>
       </c>
@@ -2035,17 +2375,23 @@
       <c r="E49" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49">
         <v>38514479</v>
       </c>
-      <c r="G49">
+      <c r="I49">
         <v>306220</v>
       </c>
-      <c r="H49" s="2">
+      <c r="J49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="15" thickBot="1">
+    <row r="50" spans="2:10" ht="15" thickBot="1">
       <c r="B50" s="1" t="s">
         <v>26</v>
       </c>
@@ -2058,12 +2404,18 @@
       <c r="E50" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F50" s="3"/>
-      <c r="H50" s="2">
+      <c r="F50" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H50" s="3"/>
+      <c r="J50" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="15" thickBot="1">
+    <row r="51" spans="2:10" ht="15" thickBot="1">
       <c r="B51" s="1" t="s">
         <v>30</v>
       </c>
@@ -2076,17 +2428,23 @@
       <c r="E51" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H51">
         <v>10457295</v>
       </c>
-      <c r="G51">
+      <c r="I51">
         <v>91590</v>
       </c>
-      <c r="H51" s="2">
+      <c r="J51" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="27" thickBot="1">
+    <row r="52" spans="2:10" ht="15" thickBot="1">
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
@@ -2099,17 +2457,23 @@
       <c r="E52" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H52">
         <v>19981358</v>
       </c>
-      <c r="G52">
+      <c r="I52">
         <v>230020</v>
       </c>
-      <c r="H52" s="2">
+      <c r="J52" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="27" thickBot="1">
+    <row r="53" spans="2:10" ht="15" thickBot="1">
       <c r="B53" s="1" t="s">
         <v>101</v>
       </c>
@@ -2122,17 +2486,23 @@
       <c r="E53" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H53">
         <v>7164132</v>
       </c>
-      <c r="G53">
+      <c r="I53">
         <v>87460</v>
       </c>
-      <c r="H53" s="2">
+      <c r="J53" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="15" thickBot="1">
+    <row r="54" spans="2:10" ht="15" thickBot="1">
       <c r="B54" s="1" t="s">
         <v>61</v>
       </c>
@@ -2145,17 +2515,23 @@
       <c r="E54" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H54">
         <v>143499861</v>
       </c>
-      <c r="G54">
+      <c r="I54">
         <v>16376870</v>
       </c>
-      <c r="H54" s="2">
+      <c r="J54" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="15" thickBot="1">
+    <row r="55" spans="2:10" ht="27" thickBot="1">
       <c r="B55" s="1" t="s">
         <v>116</v>
       </c>
@@ -2168,17 +2544,23 @@
       <c r="E55" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H55">
         <v>28828870</v>
       </c>
-      <c r="G55">
+      <c r="I55">
         <v>2149690</v>
       </c>
-      <c r="H55" s="2">
+      <c r="J55" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="15" thickBot="1">
+    <row r="56" spans="2:10" ht="15" thickBot="1">
       <c r="B56" s="1" t="s">
         <v>120</v>
       </c>
@@ -2191,17 +2573,23 @@
       <c r="E56" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H56">
         <v>9600379</v>
       </c>
-      <c r="G56">
+      <c r="I56">
         <v>407340</v>
       </c>
-      <c r="H56" s="2">
+      <c r="J56" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="15" thickBot="1">
+    <row r="57" spans="2:10" ht="15" thickBot="1">
       <c r="B57" s="1" t="s">
         <v>112</v>
       </c>
@@ -2214,17 +2602,23 @@
       <c r="E57" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H57">
         <v>2059953</v>
       </c>
-      <c r="G57">
+      <c r="I57">
         <v>20140</v>
       </c>
-      <c r="H57" s="2">
+      <c r="J57" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="15" thickBot="1">
+    <row r="58" spans="2:10" ht="15" thickBot="1">
       <c r="B58" s="1" t="s">
         <v>108</v>
       </c>
@@ -2237,17 +2631,23 @@
       <c r="E58" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H58">
         <v>5413393</v>
       </c>
-      <c r="G58">
+      <c r="I58">
         <v>48088</v>
       </c>
-      <c r="H58" s="2">
+      <c r="J58" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="27" thickBot="1">
+    <row r="59" spans="2:10" ht="15" thickBot="1">
       <c r="B59" s="1" t="s">
         <v>114</v>
       </c>
@@ -2260,17 +2660,23 @@
       <c r="E59" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H59">
         <v>31448</v>
       </c>
-      <c r="G59">
+      <c r="I59">
         <v>60</v>
       </c>
-      <c r="H59" s="2">
+      <c r="J59" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="15" thickBot="1">
+    <row r="60" spans="2:10" ht="15" thickBot="1">
       <c r="B60" s="1" t="s">
         <v>93</v>
       </c>
@@ -2283,17 +2689,23 @@
       <c r="E60" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H60">
         <v>22845550</v>
       </c>
-      <c r="G60">
+      <c r="I60">
         <v>183630</v>
       </c>
-      <c r="H60" s="2">
+      <c r="J60" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="2:8" ht="15" thickBot="1">
+    <row r="61" spans="2:10" ht="15" thickBot="1">
       <c r="B61" s="1" t="s">
         <v>95</v>
       </c>
@@ -2306,17 +2718,23 @@
       <c r="E61" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H61">
         <v>10886500</v>
       </c>
-      <c r="G61">
+      <c r="I61">
         <v>155360</v>
       </c>
-      <c r="H61" s="2">
+      <c r="J61" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="2:8" ht="15" thickBot="1">
+    <row r="62" spans="2:10" ht="15" thickBot="1">
       <c r="B62" s="1" t="s">
         <v>34</v>
       </c>
@@ -2329,17 +2747,23 @@
       <c r="E62" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H62">
         <v>74932641</v>
       </c>
-      <c r="G62">
+      <c r="I62">
         <v>769630</v>
       </c>
-      <c r="H62" s="2">
+      <c r="J62" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="15" thickBot="1">
+    <row r="63" spans="2:10" ht="15" thickBot="1">
       <c r="B63" s="1" t="s">
         <v>118</v>
       </c>
@@ -2352,17 +2776,23 @@
       <c r="E63" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H63">
         <v>45489600</v>
       </c>
-      <c r="G63">
+      <c r="I63">
         <v>579320</v>
       </c>
-      <c r="H63" s="2">
+      <c r="J63" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="26">
+    <row r="64" spans="2:10">
       <c r="B64" s="4" t="s">
         <v>132</v>
       </c>
@@ -2375,13 +2805,19 @@
       <c r="E64" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H64">
         <v>1824000</v>
       </c>
-      <c r="G64">
+      <c r="I64">
         <v>10887</v>
       </c>
-      <c r="H64" s="2">
+      <c r="J64" s="2">
         <v>32</v>
       </c>
     </row>

</xml_diff>